<commit_message>
Horas gasta par Nav e Ir ao Conteudo
</commit_message>
<xml_diff>
--- a/documento_projeto/Pixels - Orçamento de correção.xlsx
+++ b/documento_projeto/Pixels - Orçamento de correção.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Carolina\FATEC\3 Semestre\acessibilidade\semana_06\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\pixels\documento_projeto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A72783C2-E844-4B81-A671-BBA6B7C68950}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E63802C-DACC-47D2-8D95-2DE3CC99E47D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="orçamento" sheetId="4" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="114">
   <si>
     <t>ID</t>
   </si>
@@ -376,6 +376,9 @@
   <si>
     <t>Todas as paginas não possui link para no inicio para levar ao 
 conteudo h1</t>
+  </si>
+  <si>
+    <t>Tempo Gasto/min</t>
   </si>
 </sst>
 </file>
@@ -426,7 +429,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -455,6 +458,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFF99FF"/>
         <bgColor rgb="FFFF99FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -550,7 +559,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -617,9 +626,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -632,9 +638,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -682,6 +685,18 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -905,8 +920,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A045B8F-3550-4BE9-82FC-AF0F1FC4BEDF}">
   <dimension ref="A1:O72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G71" sqref="G71"/>
+    <sheetView tabSelected="1" topLeftCell="F49" workbookViewId="0">
+      <selection activeCell="M70" sqref="M70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -920,7 +935,8 @@
     <col min="7" max="7" width="17.5703125" customWidth="1"/>
     <col min="8" max="8" width="22.28515625" customWidth="1"/>
     <col min="9" max="9" width="14.85546875" customWidth="1"/>
-    <col min="10" max="12" width="11.85546875" customWidth="1"/>
+    <col min="10" max="11" width="11.85546875" customWidth="1"/>
+    <col min="12" max="12" width="17.28515625" customWidth="1"/>
     <col min="13" max="13" width="9.140625" customWidth="1"/>
     <col min="14" max="14" width="14" customWidth="1"/>
     <col min="15" max="15" width="14" bestFit="1" customWidth="1"/>
@@ -945,10 +961,10 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="43" t="s">
+      <c r="G1" s="41" t="s">
         <v>100</v>
       </c>
-      <c r="H1" s="44" t="s">
+      <c r="H1" s="42" t="s">
         <v>96</v>
       </c>
       <c r="I1" s="1" t="s">
@@ -957,14 +973,16 @@
       <c r="J1" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="46" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="31"/>
-      <c r="N1" s="39" t="s">
+      <c r="L1" s="48" t="s">
+        <v>113</v>
+      </c>
+      <c r="N1" s="37" t="s">
         <v>103</v>
       </c>
-      <c r="O1" s="36" t="s">
+      <c r="O1" s="34" t="s">
         <v>109</v>
       </c>
     </row>
@@ -990,22 +1008,24 @@
       <c r="G2" s="12">
         <v>20</v>
       </c>
-      <c r="H2" s="27">
+      <c r="H2" s="26">
         <v>360</v>
       </c>
-      <c r="I2" s="32" t="s">
+      <c r="I2" s="30" t="s">
         <v>98</v>
       </c>
-      <c r="J2" s="35">
+      <c r="J2" s="33">
         <f>H2/60</f>
         <v>6</v>
       </c>
-      <c r="K2" s="35">
+      <c r="K2" s="47">
         <f>O2*J2</f>
         <v>450</v>
       </c>
-      <c r="L2" s="26"/>
-      <c r="N2" s="40" t="s">
+      <c r="L2" s="49">
+        <v>400</v>
+      </c>
+      <c r="N2" s="38" t="s">
         <v>98</v>
       </c>
       <c r="O2" s="25">
@@ -1034,22 +1054,22 @@
       <c r="G3" s="12">
         <v>60</v>
       </c>
-      <c r="H3" s="27">
+      <c r="H3" s="26">
         <v>60</v>
       </c>
-      <c r="I3" s="33" t="s">
-        <v>99</v>
-      </c>
-      <c r="J3" s="35">
+      <c r="I3" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="J3" s="33">
         <f t="shared" ref="J3:J66" si="0">H3/60</f>
         <v>1</v>
       </c>
-      <c r="K3" s="35">
+      <c r="K3" s="47">
         <f>O4*J3</f>
         <v>52.5</v>
       </c>
-      <c r="L3" s="26"/>
-      <c r="N3" s="41" t="s">
+      <c r="L3" s="49"/>
+      <c r="N3" s="39" t="s">
         <v>106</v>
       </c>
       <c r="O3" s="25">
@@ -1078,22 +1098,22 @@
       <c r="G4" s="12">
         <v>10</v>
       </c>
-      <c r="H4" s="27">
-        <v>10</v>
-      </c>
-      <c r="I4" s="33" t="s">
-        <v>99</v>
-      </c>
-      <c r="J4" s="35">
-        <f t="shared" si="0"/>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="K4" s="35">
+      <c r="H4" s="26">
+        <v>10</v>
+      </c>
+      <c r="I4" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="J4" s="33">
+        <f t="shared" si="0"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="K4" s="47">
         <f>O5*J4</f>
         <v>10</v>
       </c>
-      <c r="L4" s="26"/>
-      <c r="N4" s="42" t="s">
+      <c r="L4" s="49"/>
+      <c r="N4" s="40" t="s">
         <v>99</v>
       </c>
       <c r="O4" s="25">
@@ -1122,22 +1142,22 @@
       <c r="G5" s="12">
         <v>10</v>
       </c>
-      <c r="H5" s="27">
-        <v>10</v>
-      </c>
-      <c r="I5" s="33" t="s">
-        <v>99</v>
-      </c>
-      <c r="J5" s="35">
-        <f t="shared" si="0"/>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="K5" s="35">
+      <c r="H5" s="26">
+        <v>10</v>
+      </c>
+      <c r="I5" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="J5" s="33">
+        <f t="shared" si="0"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="K5" s="47">
         <f>O6*J5</f>
         <v>14.25</v>
       </c>
-      <c r="L5" s="26"/>
-      <c r="N5" s="42" t="s">
+      <c r="L5" s="49"/>
+      <c r="N5" s="40" t="s">
         <v>104</v>
       </c>
       <c r="O5" s="25">
@@ -1166,21 +1186,21 @@
       <c r="G6" s="12">
         <v>15</v>
       </c>
-      <c r="H6" s="27">
+      <c r="H6" s="26">
         <v>20</v>
       </c>
-      <c r="I6" s="34" t="s">
+      <c r="I6" s="32" t="s">
         <v>106</v>
       </c>
-      <c r="J6" s="35">
+      <c r="J6" s="33">
         <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="K6" s="35">
+      <c r="K6" s="47">
         <f>O3*J6</f>
         <v>17.5</v>
       </c>
-      <c r="L6" s="26"/>
+      <c r="L6" s="49"/>
       <c r="N6" s="19" t="s">
         <v>105</v>
       </c>
@@ -1210,21 +1230,21 @@
       <c r="G7" s="12">
         <v>15</v>
       </c>
-      <c r="H7" s="27">
-        <v>10</v>
-      </c>
-      <c r="I7" s="32" t="s">
+      <c r="H7" s="26">
+        <v>10</v>
+      </c>
+      <c r="I7" s="30" t="s">
         <v>98</v>
       </c>
-      <c r="J7" s="35">
-        <f t="shared" si="0"/>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="K7" s="35">
+      <c r="J7" s="33">
+        <f t="shared" si="0"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="K7" s="47">
         <f>O2*J7</f>
         <v>12.5</v>
       </c>
-      <c r="L7" s="26"/>
+      <c r="L7" s="49"/>
     </row>
     <row r="8" spans="1:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
@@ -1248,21 +1268,21 @@
       <c r="G8" s="12">
         <v>10</v>
       </c>
-      <c r="H8" s="27">
-        <v>10</v>
-      </c>
-      <c r="I8" s="33" t="s">
-        <v>99</v>
-      </c>
-      <c r="J8" s="35">
-        <f t="shared" si="0"/>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="K8" s="35">
+      <c r="H8" s="26">
+        <v>10</v>
+      </c>
+      <c r="I8" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="J8" s="33">
+        <f t="shared" si="0"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="K8" s="47">
         <f>$O$4*J8</f>
         <v>8.75</v>
       </c>
-      <c r="L8" s="26"/>
+      <c r="L8" s="49"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
@@ -1286,21 +1306,21 @@
       <c r="G9" s="12">
         <v>10</v>
       </c>
-      <c r="H9" s="27">
-        <v>10</v>
-      </c>
-      <c r="I9" s="33" t="s">
-        <v>99</v>
-      </c>
-      <c r="J9" s="35">
-        <f t="shared" si="0"/>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="K9" s="35">
+      <c r="H9" s="26">
+        <v>10</v>
+      </c>
+      <c r="I9" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="J9" s="33">
+        <f t="shared" si="0"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="K9" s="47">
         <f t="shared" ref="K9:K21" si="1">$O$4*J9</f>
         <v>8.75</v>
       </c>
-      <c r="L9" s="26"/>
+      <c r="L9" s="49"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
@@ -1324,21 +1344,21 @@
       <c r="G10" s="12">
         <v>10</v>
       </c>
-      <c r="H10" s="27">
-        <v>10</v>
-      </c>
-      <c r="I10" s="33" t="s">
-        <v>99</v>
-      </c>
-      <c r="J10" s="35">
-        <f t="shared" si="0"/>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="K10" s="35">
+      <c r="H10" s="26">
+        <v>10</v>
+      </c>
+      <c r="I10" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="J10" s="33">
+        <f t="shared" si="0"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="K10" s="47">
         <f t="shared" si="1"/>
         <v>8.75</v>
       </c>
-      <c r="L10" s="26"/>
+      <c r="L10" s="49"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
@@ -1362,21 +1382,21 @@
       <c r="G11" s="12">
         <v>10</v>
       </c>
-      <c r="H11" s="27">
-        <v>10</v>
-      </c>
-      <c r="I11" s="33" t="s">
-        <v>99</v>
-      </c>
-      <c r="J11" s="35">
-        <f t="shared" si="0"/>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="K11" s="35">
+      <c r="H11" s="26">
+        <v>10</v>
+      </c>
+      <c r="I11" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="J11" s="33">
+        <f t="shared" si="0"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="K11" s="47">
         <f t="shared" si="1"/>
         <v>8.75</v>
       </c>
-      <c r="L11" s="26"/>
+      <c r="L11" s="49"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
@@ -1400,21 +1420,21 @@
       <c r="G12" s="12">
         <v>10</v>
       </c>
-      <c r="H12" s="27">
-        <v>10</v>
-      </c>
-      <c r="I12" s="33" t="s">
-        <v>99</v>
-      </c>
-      <c r="J12" s="35">
-        <f t="shared" si="0"/>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="K12" s="35">
+      <c r="H12" s="26">
+        <v>10</v>
+      </c>
+      <c r="I12" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="J12" s="33">
+        <f t="shared" si="0"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="K12" s="47">
         <f t="shared" si="1"/>
         <v>8.75</v>
       </c>
-      <c r="L12" s="26"/>
+      <c r="L12" s="49"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
@@ -1438,21 +1458,21 @@
       <c r="G13" s="12">
         <v>10</v>
       </c>
-      <c r="H13" s="27">
-        <v>10</v>
-      </c>
-      <c r="I13" s="33" t="s">
-        <v>99</v>
-      </c>
-      <c r="J13" s="35">
-        <f t="shared" si="0"/>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="K13" s="35">
+      <c r="H13" s="26">
+        <v>10</v>
+      </c>
+      <c r="I13" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="J13" s="33">
+        <f t="shared" si="0"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="K13" s="47">
         <f t="shared" si="1"/>
         <v>8.75</v>
       </c>
-      <c r="L13" s="26"/>
+      <c r="L13" s="49"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
@@ -1476,21 +1496,21 @@
       <c r="G14" s="12">
         <v>15</v>
       </c>
-      <c r="H14" s="27">
-        <v>10</v>
-      </c>
-      <c r="I14" s="33" t="s">
-        <v>99</v>
-      </c>
-      <c r="J14" s="35">
-        <f t="shared" si="0"/>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="K14" s="35">
+      <c r="H14" s="26">
+        <v>10</v>
+      </c>
+      <c r="I14" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="J14" s="33">
+        <f t="shared" si="0"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="K14" s="47">
         <f t="shared" si="1"/>
         <v>8.75</v>
       </c>
-      <c r="L14" s="26"/>
+      <c r="L14" s="49"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
@@ -1514,21 +1534,21 @@
       <c r="G15" s="12">
         <v>15</v>
       </c>
-      <c r="H15" s="27">
-        <v>10</v>
-      </c>
-      <c r="I15" s="33" t="s">
-        <v>99</v>
-      </c>
-      <c r="J15" s="35">
-        <f t="shared" si="0"/>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="K15" s="35">
+      <c r="H15" s="26">
+        <v>10</v>
+      </c>
+      <c r="I15" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="J15" s="33">
+        <f t="shared" si="0"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="K15" s="47">
         <f t="shared" si="1"/>
         <v>8.75</v>
       </c>
-      <c r="L15" s="26"/>
+      <c r="L15" s="49"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
@@ -1552,21 +1572,21 @@
       <c r="G16" s="12">
         <v>10</v>
       </c>
-      <c r="H16" s="27">
-        <v>10</v>
-      </c>
-      <c r="I16" s="33" t="s">
-        <v>99</v>
-      </c>
-      <c r="J16" s="35">
-        <f t="shared" si="0"/>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="K16" s="35">
+      <c r="H16" s="26">
+        <v>10</v>
+      </c>
+      <c r="I16" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="J16" s="33">
+        <f t="shared" si="0"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="K16" s="47">
         <f t="shared" si="1"/>
         <v>8.75</v>
       </c>
-      <c r="L16" s="26"/>
+      <c r="L16" s="49"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
@@ -1590,21 +1610,21 @@
       <c r="G17" s="12">
         <v>10</v>
       </c>
-      <c r="H17" s="27">
-        <v>10</v>
-      </c>
-      <c r="I17" s="33" t="s">
-        <v>99</v>
-      </c>
-      <c r="J17" s="35">
-        <f t="shared" si="0"/>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="K17" s="35">
+      <c r="H17" s="26">
+        <v>10</v>
+      </c>
+      <c r="I17" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="J17" s="33">
+        <f t="shared" si="0"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="K17" s="47">
         <f t="shared" si="1"/>
         <v>8.75</v>
       </c>
-      <c r="L17" s="26"/>
+      <c r="L17" s="49"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
@@ -1628,21 +1648,21 @@
       <c r="G18" s="12">
         <v>10</v>
       </c>
-      <c r="H18" s="27">
-        <v>10</v>
-      </c>
-      <c r="I18" s="33" t="s">
-        <v>99</v>
-      </c>
-      <c r="J18" s="35">
-        <f t="shared" si="0"/>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="K18" s="35">
+      <c r="H18" s="26">
+        <v>10</v>
+      </c>
+      <c r="I18" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="J18" s="33">
+        <f t="shared" si="0"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="K18" s="47">
         <f t="shared" si="1"/>
         <v>8.75</v>
       </c>
-      <c r="L18" s="26"/>
+      <c r="L18" s="49"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
@@ -1666,21 +1686,21 @@
       <c r="G19" s="12">
         <v>10</v>
       </c>
-      <c r="H19" s="27">
-        <v>10</v>
-      </c>
-      <c r="I19" s="33" t="s">
-        <v>99</v>
-      </c>
-      <c r="J19" s="35">
-        <f t="shared" si="0"/>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="K19" s="35">
+      <c r="H19" s="26">
+        <v>10</v>
+      </c>
+      <c r="I19" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="J19" s="33">
+        <f t="shared" si="0"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="K19" s="47">
         <f t="shared" si="1"/>
         <v>8.75</v>
       </c>
-      <c r="L19" s="26"/>
+      <c r="L19" s="49"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
@@ -1704,21 +1724,21 @@
       <c r="G20" s="12">
         <v>10</v>
       </c>
-      <c r="H20" s="27">
-        <v>10</v>
-      </c>
-      <c r="I20" s="33" t="s">
-        <v>99</v>
-      </c>
-      <c r="J20" s="35">
-        <f t="shared" si="0"/>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="K20" s="35">
+      <c r="H20" s="26">
+        <v>10</v>
+      </c>
+      <c r="I20" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="J20" s="33">
+        <f t="shared" si="0"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="K20" s="47">
         <f t="shared" si="1"/>
         <v>8.75</v>
       </c>
-      <c r="L20" s="26"/>
+      <c r="L20" s="49"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
@@ -1742,21 +1762,21 @@
       <c r="G21" s="12">
         <v>15</v>
       </c>
-      <c r="H21" s="27">
-        <v>10</v>
-      </c>
-      <c r="I21" s="33" t="s">
-        <v>99</v>
-      </c>
-      <c r="J21" s="35">
-        <f t="shared" si="0"/>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="K21" s="35">
+      <c r="H21" s="26">
+        <v>10</v>
+      </c>
+      <c r="I21" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="J21" s="33">
+        <f t="shared" si="0"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="K21" s="47">
         <f t="shared" si="1"/>
         <v>8.75</v>
       </c>
-      <c r="L21" s="26"/>
+      <c r="L21" s="49"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
@@ -1780,21 +1800,21 @@
       <c r="G22" s="12">
         <v>15</v>
       </c>
-      <c r="H22" s="27">
+      <c r="H22" s="26">
         <v>15</v>
       </c>
-      <c r="I22" s="32" t="s">
+      <c r="I22" s="30" t="s">
         <v>98</v>
       </c>
-      <c r="J22" s="35">
+      <c r="J22" s="33">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-      <c r="K22" s="35">
+      <c r="K22" s="47">
         <f>$O$2*J22</f>
         <v>18.75</v>
       </c>
-      <c r="L22" s="26"/>
+      <c r="L22" s="49"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
@@ -1818,21 +1838,21 @@
       <c r="G23" s="12">
         <v>15</v>
       </c>
-      <c r="H23" s="27">
+      <c r="H23" s="26">
         <v>15</v>
       </c>
-      <c r="I23" s="32" t="s">
+      <c r="I23" s="30" t="s">
         <v>98</v>
       </c>
-      <c r="J23" s="35">
+      <c r="J23" s="33">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-      <c r="K23" s="35">
+      <c r="K23" s="47">
         <f t="shared" ref="K23:K25" si="2">$O$2*J23</f>
         <v>18.75</v>
       </c>
-      <c r="L23" s="26"/>
+      <c r="L23" s="49"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
@@ -1856,21 +1876,21 @@
       <c r="G24" s="12">
         <v>30</v>
       </c>
-      <c r="H24" s="27">
+      <c r="H24" s="26">
         <v>15</v>
       </c>
-      <c r="I24" s="32" t="s">
+      <c r="I24" s="30" t="s">
         <v>98</v>
       </c>
-      <c r="J24" s="35">
+      <c r="J24" s="33">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-      <c r="K24" s="35">
+      <c r="K24" s="47">
         <f t="shared" si="2"/>
         <v>18.75</v>
       </c>
-      <c r="L24" s="26"/>
+      <c r="L24" s="49"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
@@ -1882,10 +1902,10 @@
       <c r="C25" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="D25" s="38" t="s">
+      <c r="D25" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="E25" s="38" t="s">
+      <c r="E25" s="36" t="s">
         <v>9</v>
       </c>
       <c r="F25" s="9" t="s">
@@ -1894,21 +1914,21 @@
       <c r="G25" s="12">
         <v>30</v>
       </c>
-      <c r="H25" s="27">
+      <c r="H25" s="26">
         <v>15</v>
       </c>
-      <c r="I25" s="32" t="s">
+      <c r="I25" s="30" t="s">
         <v>98</v>
       </c>
-      <c r="J25" s="35">
+      <c r="J25" s="33">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-      <c r="K25" s="35">
+      <c r="K25" s="47">
         <f t="shared" si="2"/>
         <v>18.75</v>
       </c>
-      <c r="L25" s="26"/>
+      <c r="L25" s="49"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
@@ -1920,10 +1940,10 @@
       <c r="C26" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="D26" s="38" t="s">
+      <c r="D26" s="36" t="s">
         <v>50</v>
       </c>
-      <c r="E26" s="38" t="s">
+      <c r="E26" s="36" t="s">
         <v>9</v>
       </c>
       <c r="F26" s="9" t="s">
@@ -1932,21 +1952,21 @@
       <c r="G26" s="13">
         <v>20</v>
       </c>
-      <c r="H26" s="28">
+      <c r="H26" s="27">
         <v>20</v>
       </c>
-      <c r="I26" s="34" t="s">
+      <c r="I26" s="32" t="s">
         <v>106</v>
       </c>
-      <c r="J26" s="35">
+      <c r="J26" s="33">
         <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="K26" s="35">
+      <c r="K26" s="47">
         <f>O3*J26</f>
         <v>17.5</v>
       </c>
-      <c r="L26" s="26"/>
+      <c r="L26" s="49"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
@@ -1958,10 +1978,10 @@
       <c r="C27" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="D27" s="38" t="s">
+      <c r="D27" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="E27" s="38" t="s">
+      <c r="E27" s="36" t="s">
         <v>52</v>
       </c>
       <c r="F27" s="9" t="s">
@@ -1970,21 +1990,21 @@
       <c r="G27" s="13">
         <v>15</v>
       </c>
-      <c r="H27" s="28">
-        <v>10</v>
-      </c>
-      <c r="I27" s="33" t="s">
-        <v>99</v>
-      </c>
-      <c r="J27" s="35">
-        <f t="shared" si="0"/>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="K27" s="35">
+      <c r="H27" s="27">
+        <v>10</v>
+      </c>
+      <c r="I27" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="J27" s="33">
+        <f t="shared" si="0"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="K27" s="47">
         <f>$O$4*J27</f>
         <v>8.75</v>
       </c>
-      <c r="L27" s="26"/>
+      <c r="L27" s="49"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
@@ -1996,10 +2016,10 @@
       <c r="C28" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="D28" s="38" t="s">
+      <c r="D28" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="E28" s="38" t="s">
+      <c r="E28" s="36" t="s">
         <v>54</v>
       </c>
       <c r="F28" s="9" t="s">
@@ -2008,21 +2028,21 @@
       <c r="G28" s="13">
         <v>15</v>
       </c>
-      <c r="H28" s="28">
-        <v>10</v>
-      </c>
-      <c r="I28" s="33" t="s">
-        <v>99</v>
-      </c>
-      <c r="J28" s="35">
-        <f t="shared" si="0"/>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="K28" s="35">
+      <c r="H28" s="27">
+        <v>10</v>
+      </c>
+      <c r="I28" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="J28" s="33">
+        <f t="shared" si="0"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="K28" s="47">
         <f t="shared" ref="K28:K30" si="3">$O$4*J28</f>
         <v>8.75</v>
       </c>
-      <c r="L28" s="26"/>
+      <c r="L28" s="49"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
@@ -2034,10 +2054,10 @@
       <c r="C29" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="D29" s="38" t="s">
+      <c r="D29" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="E29" s="38" t="s">
+      <c r="E29" s="36" t="s">
         <v>39</v>
       </c>
       <c r="F29" s="9" t="s">
@@ -2046,21 +2066,21 @@
       <c r="G29" s="13">
         <v>15</v>
       </c>
-      <c r="H29" s="28">
-        <v>10</v>
-      </c>
-      <c r="I29" s="33" t="s">
-        <v>99</v>
-      </c>
-      <c r="J29" s="35">
-        <f t="shared" si="0"/>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="K29" s="35">
+      <c r="H29" s="27">
+        <v>10</v>
+      </c>
+      <c r="I29" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="J29" s="33">
+        <f t="shared" si="0"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="K29" s="47">
         <f t="shared" si="3"/>
         <v>8.75</v>
       </c>
-      <c r="L29" s="26"/>
+      <c r="L29" s="49"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
@@ -2072,10 +2092,10 @@
       <c r="C30" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="D30" s="38" t="s">
+      <c r="D30" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="E30" s="38" t="s">
+      <c r="E30" s="36" t="s">
         <v>55</v>
       </c>
       <c r="F30" s="9" t="s">
@@ -2084,21 +2104,21 @@
       <c r="G30" s="13">
         <v>15</v>
       </c>
-      <c r="H30" s="28">
-        <v>10</v>
-      </c>
-      <c r="I30" s="33" t="s">
-        <v>99</v>
-      </c>
-      <c r="J30" s="35">
-        <f t="shared" si="0"/>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="K30" s="35">
+      <c r="H30" s="27">
+        <v>10</v>
+      </c>
+      <c r="I30" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="J30" s="33">
+        <f t="shared" si="0"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="K30" s="47">
         <f t="shared" si="3"/>
         <v>8.75</v>
       </c>
-      <c r="L30" s="26"/>
+      <c r="L30" s="49"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
@@ -2110,10 +2130,10 @@
       <c r="C31" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="D31" s="38" t="s">
+      <c r="D31" s="36" t="s">
         <v>56</v>
       </c>
-      <c r="E31" s="38" t="s">
+      <c r="E31" s="36" t="s">
         <v>37</v>
       </c>
       <c r="F31" s="9" t="s">
@@ -2122,21 +2142,21 @@
       <c r="G31" s="13">
         <v>10</v>
       </c>
-      <c r="H31" s="28">
+      <c r="H31" s="27">
         <v>15</v>
       </c>
-      <c r="I31" s="34" t="s">
+      <c r="I31" s="32" t="s">
         <v>106</v>
       </c>
-      <c r="J31" s="35">
+      <c r="J31" s="33">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-      <c r="K31" s="35">
+      <c r="K31" s="47">
         <f>O3*J31</f>
         <v>13.125</v>
       </c>
-      <c r="L31" s="26"/>
+      <c r="L31" s="49"/>
     </row>
     <row r="32" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
@@ -2148,33 +2168,33 @@
       <c r="C32" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="D32" s="38" t="s">
+      <c r="D32" s="36" t="s">
         <v>58</v>
       </c>
-      <c r="E32" s="38" t="s">
+      <c r="E32" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="F32" s="45" t="s">
+      <c r="F32" s="43" t="s">
         <v>60</v>
       </c>
       <c r="G32" s="13">
         <v>10</v>
       </c>
-      <c r="H32" s="28">
+      <c r="H32" s="27">
         <v>15</v>
       </c>
-      <c r="I32" s="33" t="s">
-        <v>99</v>
-      </c>
-      <c r="J32" s="35">
+      <c r="I32" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="J32" s="33">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-      <c r="K32" s="35">
+      <c r="K32" s="47">
         <f>$O$4*J32</f>
         <v>13.125</v>
       </c>
-      <c r="L32" s="26"/>
+      <c r="L32" s="49"/>
     </row>
     <row r="33" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
@@ -2186,33 +2206,33 @@
       <c r="C33" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="D33" s="38" t="s">
+      <c r="D33" s="36" t="s">
         <v>58</v>
       </c>
-      <c r="E33" s="38" t="s">
+      <c r="E33" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="F33" s="45" t="s">
+      <c r="F33" s="43" t="s">
         <v>61</v>
       </c>
       <c r="G33" s="13">
         <v>10</v>
       </c>
-      <c r="H33" s="28">
+      <c r="H33" s="27">
         <v>15</v>
       </c>
-      <c r="I33" s="33" t="s">
-        <v>99</v>
-      </c>
-      <c r="J33" s="35">
+      <c r="I33" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="J33" s="33">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-      <c r="K33" s="35">
+      <c r="K33" s="47">
         <f>$O$4*J33</f>
         <v>13.125</v>
       </c>
-      <c r="L33" s="26"/>
+      <c r="L33" s="49"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
@@ -2236,21 +2256,21 @@
       <c r="G34" s="12">
         <v>10</v>
       </c>
-      <c r="H34" s="27">
+      <c r="H34" s="26">
         <v>60</v>
       </c>
-      <c r="I34" s="32" t="s">
+      <c r="I34" s="30" t="s">
         <v>98</v>
       </c>
-      <c r="J34" s="35">
+      <c r="J34" s="33">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="K34" s="35">
+      <c r="K34" s="47">
         <f>$O$2*J34</f>
         <v>75</v>
       </c>
-      <c r="L34" s="26"/>
+      <c r="L34" s="49"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
@@ -2262,10 +2282,10 @@
       <c r="C35" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="D35" s="38" t="s">
+      <c r="D35" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="E35" s="38" t="s">
+      <c r="E35" s="36" t="s">
         <v>9</v>
       </c>
       <c r="F35" s="9" t="s">
@@ -2274,21 +2294,21 @@
       <c r="G35" s="12">
         <v>10</v>
       </c>
-      <c r="H35" s="27">
+      <c r="H35" s="26">
         <v>30</v>
       </c>
-      <c r="I35" s="32" t="s">
+      <c r="I35" s="30" t="s">
         <v>98</v>
       </c>
-      <c r="J35" s="35">
+      <c r="J35" s="33">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="K35" s="35">
+      <c r="K35" s="47">
         <f t="shared" ref="K35:K37" si="4">$O$2*J35</f>
         <v>37.5</v>
       </c>
-      <c r="L35" s="26"/>
+      <c r="L35" s="49"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
@@ -2312,21 +2332,21 @@
       <c r="G36" s="12">
         <v>10</v>
       </c>
-      <c r="H36" s="27">
+      <c r="H36" s="26">
         <v>30</v>
       </c>
-      <c r="I36" s="32" t="s">
+      <c r="I36" s="30" t="s">
         <v>98</v>
       </c>
-      <c r="J36" s="35">
+      <c r="J36" s="33">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="K36" s="35">
+      <c r="K36" s="47">
         <f t="shared" si="4"/>
         <v>37.5</v>
       </c>
-      <c r="L36" s="26"/>
+      <c r="L36" s="49"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
@@ -2350,21 +2370,21 @@
       <c r="G37" s="12">
         <v>10</v>
       </c>
-      <c r="H37" s="27">
+      <c r="H37" s="26">
         <v>30</v>
       </c>
-      <c r="I37" s="32" t="s">
+      <c r="I37" s="30" t="s">
         <v>98</v>
       </c>
-      <c r="J37" s="35">
+      <c r="J37" s="33">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="K37" s="35">
+      <c r="K37" s="47">
         <f t="shared" si="4"/>
         <v>37.5</v>
       </c>
-      <c r="L37" s="26"/>
+      <c r="L37" s="49"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
@@ -2388,21 +2408,21 @@
       <c r="G38" s="12">
         <v>10</v>
       </c>
-      <c r="H38" s="27">
+      <c r="H38" s="26">
         <v>20</v>
       </c>
-      <c r="I38" s="33" t="s">
-        <v>99</v>
-      </c>
-      <c r="J38" s="35">
+      <c r="I38" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="J38" s="33">
         <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="K38" s="35">
+      <c r="K38" s="47">
         <f>$O$4*J38</f>
         <v>17.5</v>
       </c>
-      <c r="L38" s="26"/>
+      <c r="L38" s="49"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
@@ -2426,21 +2446,21 @@
       <c r="G39" s="12">
         <v>10</v>
       </c>
-      <c r="H39" s="27">
+      <c r="H39" s="26">
         <v>20</v>
       </c>
-      <c r="I39" s="33" t="s">
-        <v>99</v>
-      </c>
-      <c r="J39" s="35">
+      <c r="I39" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="J39" s="33">
         <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="K39" s="35">
+      <c r="K39" s="47">
         <f t="shared" ref="K39:K41" si="5">$O$4*J39</f>
         <v>17.5</v>
       </c>
-      <c r="L39" s="26"/>
+      <c r="L39" s="49"/>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
@@ -2464,21 +2484,21 @@
       <c r="G40" s="12">
         <v>10</v>
       </c>
-      <c r="H40" s="27">
+      <c r="H40" s="26">
         <v>60</v>
       </c>
-      <c r="I40" s="33" t="s">
-        <v>99</v>
-      </c>
-      <c r="J40" s="35">
+      <c r="I40" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="J40" s="33">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="K40" s="35">
+      <c r="K40" s="47">
         <f t="shared" si="5"/>
         <v>52.5</v>
       </c>
-      <c r="L40" s="26"/>
+      <c r="L40" s="49"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
@@ -2502,21 +2522,21 @@
       <c r="G41" s="12">
         <v>10</v>
       </c>
-      <c r="H41" s="27">
+      <c r="H41" s="26">
         <v>60</v>
       </c>
-      <c r="I41" s="33" t="s">
-        <v>99</v>
-      </c>
-      <c r="J41" s="35">
+      <c r="I41" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="J41" s="33">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="K41" s="35">
+      <c r="K41" s="47">
         <f t="shared" si="5"/>
         <v>52.5</v>
       </c>
-      <c r="L41" s="26"/>
+      <c r="L41" s="49"/>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
@@ -2540,21 +2560,21 @@
       <c r="G42" s="12">
         <v>10</v>
       </c>
-      <c r="H42" s="27">
+      <c r="H42" s="26">
         <v>15</v>
       </c>
-      <c r="I42" s="34" t="s">
+      <c r="I42" s="32" t="s">
         <v>106</v>
       </c>
-      <c r="J42" s="35">
+      <c r="J42" s="33">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-      <c r="K42" s="35">
+      <c r="K42" s="47">
         <f>$O$3*J42</f>
         <v>13.125</v>
       </c>
-      <c r="L42" s="26"/>
+      <c r="L42" s="49"/>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
@@ -2578,21 +2598,21 @@
       <c r="G43" s="12">
         <v>10</v>
       </c>
-      <c r="H43" s="27">
+      <c r="H43" s="26">
         <v>20</v>
       </c>
-      <c r="I43" s="34" t="s">
+      <c r="I43" s="32" t="s">
         <v>106</v>
       </c>
-      <c r="J43" s="35">
+      <c r="J43" s="33">
         <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="K43" s="35">
+      <c r="K43" s="47">
         <f t="shared" ref="K43:K44" si="6">$O$3*J43</f>
         <v>17.5</v>
       </c>
-      <c r="L43" s="26"/>
+      <c r="L43" s="49"/>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
@@ -2616,21 +2636,21 @@
       <c r="G44" s="12">
         <v>10</v>
       </c>
-      <c r="H44" s="27">
+      <c r="H44" s="26">
         <v>20</v>
       </c>
-      <c r="I44" s="34" t="s">
+      <c r="I44" s="32" t="s">
         <v>106</v>
       </c>
-      <c r="J44" s="35">
+      <c r="J44" s="33">
         <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="K44" s="35">
+      <c r="K44" s="47">
         <f t="shared" si="6"/>
         <v>17.5</v>
       </c>
-      <c r="L44" s="26"/>
+      <c r="L44" s="49"/>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
@@ -2654,21 +2674,21 @@
       <c r="G45" s="12">
         <v>10</v>
       </c>
-      <c r="H45" s="27">
-        <v>10</v>
-      </c>
-      <c r="I45" s="33" t="s">
-        <v>99</v>
-      </c>
-      <c r="J45" s="35">
-        <f t="shared" si="0"/>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="K45" s="35">
+      <c r="H45" s="26">
+        <v>10</v>
+      </c>
+      <c r="I45" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="J45" s="33">
+        <f t="shared" si="0"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="K45" s="47">
         <f>$O$4*J45</f>
         <v>8.75</v>
       </c>
-      <c r="L45" s="26"/>
+      <c r="L45" s="49"/>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
@@ -2692,21 +2712,21 @@
       <c r="G46" s="12">
         <v>10</v>
       </c>
-      <c r="H46" s="27">
-        <v>10</v>
-      </c>
-      <c r="I46" s="33" t="s">
-        <v>99</v>
-      </c>
-      <c r="J46" s="35">
-        <f t="shared" si="0"/>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="K46" s="35">
+      <c r="H46" s="26">
+        <v>10</v>
+      </c>
+      <c r="I46" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="J46" s="33">
+        <f t="shared" si="0"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="K46" s="47">
         <f t="shared" ref="K46:K49" si="7">$O$4*J46</f>
         <v>8.75</v>
       </c>
-      <c r="L46" s="26"/>
+      <c r="L46" s="49"/>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
@@ -2730,21 +2750,21 @@
       <c r="G47" s="12">
         <v>10</v>
       </c>
-      <c r="H47" s="27">
-        <v>10</v>
-      </c>
-      <c r="I47" s="33" t="s">
-        <v>99</v>
-      </c>
-      <c r="J47" s="35">
-        <f t="shared" si="0"/>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="K47" s="35">
+      <c r="H47" s="26">
+        <v>10</v>
+      </c>
+      <c r="I47" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="J47" s="33">
+        <f t="shared" si="0"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="K47" s="47">
         <f t="shared" si="7"/>
         <v>8.75</v>
       </c>
-      <c r="L47" s="26"/>
+      <c r="L47" s="49"/>
     </row>
     <row r="48" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
@@ -2762,27 +2782,27 @@
       <c r="E48" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F48" s="46" t="s">
+      <c r="F48" s="44" t="s">
         <v>111</v>
       </c>
       <c r="G48" s="12">
         <v>10</v>
       </c>
-      <c r="H48" s="27">
+      <c r="H48" s="26">
         <v>15</v>
       </c>
-      <c r="I48" s="33" t="s">
-        <v>99</v>
-      </c>
-      <c r="J48" s="35">
+      <c r="I48" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="J48" s="33">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-      <c r="K48" s="35">
+      <c r="K48" s="47">
         <f t="shared" si="7"/>
         <v>13.125</v>
       </c>
-      <c r="L48" s="26"/>
+      <c r="L48" s="49"/>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
@@ -2806,21 +2826,21 @@
       <c r="G49" s="12">
         <v>20</v>
       </c>
-      <c r="H49" s="27">
-        <v>10</v>
-      </c>
-      <c r="I49" s="33" t="s">
-        <v>99</v>
-      </c>
-      <c r="J49" s="35">
-        <f t="shared" si="0"/>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="K49" s="35">
+      <c r="H49" s="26">
+        <v>10</v>
+      </c>
+      <c r="I49" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="J49" s="33">
+        <f t="shared" si="0"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="K49" s="47">
         <f t="shared" si="7"/>
         <v>8.75</v>
       </c>
-      <c r="L49" s="26"/>
+      <c r="L49" s="49"/>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
@@ -2844,21 +2864,21 @@
       <c r="G50" s="12">
         <v>10</v>
       </c>
-      <c r="H50" s="27">
-        <v>10</v>
-      </c>
-      <c r="I50" s="34" t="s">
+      <c r="H50" s="26">
+        <v>10</v>
+      </c>
+      <c r="I50" s="32" t="s">
         <v>106</v>
       </c>
-      <c r="J50" s="35">
-        <f t="shared" si="0"/>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="K50" s="35">
+      <c r="J50" s="33">
+        <f t="shared" si="0"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="K50" s="47">
         <f>O3*J50</f>
         <v>8.75</v>
       </c>
-      <c r="L50" s="26"/>
+      <c r="L50" s="49"/>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
@@ -2882,21 +2902,21 @@
       <c r="G51" s="12">
         <v>10</v>
       </c>
-      <c r="H51" s="27">
-        <v>10</v>
-      </c>
-      <c r="I51" s="33" t="s">
-        <v>99</v>
-      </c>
-      <c r="J51" s="35">
-        <f t="shared" si="0"/>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="K51" s="35">
+      <c r="H51" s="26">
+        <v>10</v>
+      </c>
+      <c r="I51" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="J51" s="33">
+        <f t="shared" si="0"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="K51" s="47">
         <f>$O$4*J51</f>
         <v>8.75</v>
       </c>
-      <c r="L51" s="26"/>
+      <c r="L51" s="49"/>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
@@ -2920,21 +2940,21 @@
       <c r="G52" s="12">
         <v>10</v>
       </c>
-      <c r="H52" s="27">
-        <v>10</v>
-      </c>
-      <c r="I52" s="33" t="s">
-        <v>99</v>
-      </c>
-      <c r="J52" s="35">
-        <f t="shared" si="0"/>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="K52" s="35">
+      <c r="H52" s="26">
+        <v>10</v>
+      </c>
+      <c r="I52" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="J52" s="33">
+        <f t="shared" si="0"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="K52" s="47">
         <f t="shared" ref="K52:K67" si="8">$O$4*J52</f>
         <v>8.75</v>
       </c>
-      <c r="L52" s="26"/>
+      <c r="L52" s="49"/>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
@@ -2958,21 +2978,21 @@
       <c r="G53" s="12">
         <v>15</v>
       </c>
-      <c r="H53" s="27">
+      <c r="H53" s="26">
         <v>15</v>
       </c>
-      <c r="I53" s="33" t="s">
-        <v>99</v>
-      </c>
-      <c r="J53" s="35">
+      <c r="I53" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="J53" s="33">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-      <c r="K53" s="35">
+      <c r="K53" s="47">
         <f t="shared" si="8"/>
         <v>13.125</v>
       </c>
-      <c r="L53" s="26"/>
+      <c r="L53" s="49"/>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
@@ -2996,21 +3016,21 @@
       <c r="G54" s="12">
         <v>10</v>
       </c>
-      <c r="H54" s="27">
-        <v>10</v>
-      </c>
-      <c r="I54" s="33" t="s">
-        <v>99</v>
-      </c>
-      <c r="J54" s="35">
-        <f t="shared" si="0"/>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="K54" s="35">
+      <c r="H54" s="26">
+        <v>10</v>
+      </c>
+      <c r="I54" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="J54" s="33">
+        <f t="shared" si="0"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="K54" s="47">
         <f t="shared" si="8"/>
         <v>8.75</v>
       </c>
-      <c r="L54" s="26"/>
+      <c r="L54" s="49"/>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
@@ -3034,21 +3054,21 @@
       <c r="G55" s="12">
         <v>10</v>
       </c>
-      <c r="H55" s="27">
-        <v>10</v>
-      </c>
-      <c r="I55" s="33" t="s">
-        <v>99</v>
-      </c>
-      <c r="J55" s="35">
-        <f t="shared" si="0"/>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="K55" s="35">
+      <c r="H55" s="26">
+        <v>10</v>
+      </c>
+      <c r="I55" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="J55" s="33">
+        <f t="shared" si="0"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="K55" s="47">
         <f t="shared" si="8"/>
         <v>8.75</v>
       </c>
-      <c r="L55" s="26"/>
+      <c r="L55" s="49"/>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
@@ -3072,21 +3092,21 @@
       <c r="G56" s="12">
         <v>10</v>
       </c>
-      <c r="H56" s="27">
-        <v>10</v>
-      </c>
-      <c r="I56" s="33" t="s">
-        <v>99</v>
-      </c>
-      <c r="J56" s="35">
-        <f t="shared" si="0"/>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="K56" s="35">
+      <c r="H56" s="26">
+        <v>10</v>
+      </c>
+      <c r="I56" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="J56" s="33">
+        <f t="shared" si="0"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="K56" s="47">
         <f t="shared" si="8"/>
         <v>8.75</v>
       </c>
-      <c r="L56" s="26"/>
+      <c r="L56" s="49"/>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
@@ -3110,21 +3130,21 @@
       <c r="G57" s="12">
         <v>10</v>
       </c>
-      <c r="H57" s="27">
-        <v>10</v>
-      </c>
-      <c r="I57" s="33" t="s">
-        <v>99</v>
-      </c>
-      <c r="J57" s="35">
-        <f t="shared" si="0"/>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="K57" s="35">
+      <c r="H57" s="26">
+        <v>10</v>
+      </c>
+      <c r="I57" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="J57" s="33">
+        <f t="shared" si="0"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="K57" s="47">
         <f t="shared" si="8"/>
         <v>8.75</v>
       </c>
-      <c r="L57" s="26"/>
+      <c r="L57" s="49"/>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
@@ -3148,21 +3168,21 @@
       <c r="G58" s="12">
         <v>15</v>
       </c>
-      <c r="H58" s="27">
-        <v>10</v>
-      </c>
-      <c r="I58" s="33" t="s">
-        <v>99</v>
-      </c>
-      <c r="J58" s="35">
-        <f t="shared" si="0"/>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="K58" s="35">
+      <c r="H58" s="26">
+        <v>10</v>
+      </c>
+      <c r="I58" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="J58" s="33">
+        <f t="shared" si="0"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="K58" s="47">
         <f t="shared" si="8"/>
         <v>8.75</v>
       </c>
-      <c r="L58" s="26"/>
+      <c r="L58" s="49"/>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
@@ -3186,21 +3206,21 @@
       <c r="G59" s="12">
         <v>10</v>
       </c>
-      <c r="H59" s="27">
-        <v>10</v>
-      </c>
-      <c r="I59" s="33" t="s">
-        <v>99</v>
-      </c>
-      <c r="J59" s="35">
-        <f t="shared" si="0"/>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="K59" s="35">
+      <c r="H59" s="26">
+        <v>10</v>
+      </c>
+      <c r="I59" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="J59" s="33">
+        <f t="shared" si="0"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="K59" s="47">
         <f t="shared" si="8"/>
         <v>8.75</v>
       </c>
-      <c r="L59" s="26"/>
+      <c r="L59" s="49"/>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A60" s="2">
@@ -3224,21 +3244,21 @@
       <c r="G60" s="12">
         <v>15</v>
       </c>
-      <c r="H60" s="27">
-        <v>10</v>
-      </c>
-      <c r="I60" s="33" t="s">
-        <v>99</v>
-      </c>
-      <c r="J60" s="35">
-        <f t="shared" si="0"/>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="K60" s="35">
+      <c r="H60" s="26">
+        <v>10</v>
+      </c>
+      <c r="I60" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="J60" s="33">
+        <f t="shared" si="0"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="K60" s="47">
         <f t="shared" si="8"/>
         <v>8.75</v>
       </c>
-      <c r="L60" s="26"/>
+      <c r="L60" s="49"/>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A61" s="2">
@@ -3262,21 +3282,21 @@
       <c r="G61" s="12">
         <v>15</v>
       </c>
-      <c r="H61" s="27">
-        <v>10</v>
-      </c>
-      <c r="I61" s="33" t="s">
-        <v>99</v>
-      </c>
-      <c r="J61" s="35">
-        <f t="shared" si="0"/>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="K61" s="35">
+      <c r="H61" s="26">
+        <v>10</v>
+      </c>
+      <c r="I61" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="J61" s="33">
+        <f t="shared" si="0"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="K61" s="47">
         <f t="shared" si="8"/>
         <v>8.75</v>
       </c>
-      <c r="L61" s="26"/>
+      <c r="L61" s="49"/>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A62" s="2">
@@ -3300,21 +3320,21 @@
       <c r="G62" s="12">
         <v>10</v>
       </c>
-      <c r="H62" s="27">
-        <v>10</v>
-      </c>
-      <c r="I62" s="33" t="s">
-        <v>99</v>
-      </c>
-      <c r="J62" s="35">
-        <f t="shared" si="0"/>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="K62" s="35">
+      <c r="H62" s="26">
+        <v>10</v>
+      </c>
+      <c r="I62" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="J62" s="33">
+        <f t="shared" si="0"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="K62" s="47">
         <f t="shared" si="8"/>
         <v>8.75</v>
       </c>
-      <c r="L62" s="26"/>
+      <c r="L62" s="49"/>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A63" s="2">
@@ -3338,21 +3358,21 @@
       <c r="G63" s="12">
         <v>10</v>
       </c>
-      <c r="H63" s="27">
-        <v>10</v>
-      </c>
-      <c r="I63" s="33" t="s">
-        <v>99</v>
-      </c>
-      <c r="J63" s="35">
-        <f t="shared" si="0"/>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="K63" s="35">
+      <c r="H63" s="26">
+        <v>10</v>
+      </c>
+      <c r="I63" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="J63" s="33">
+        <f t="shared" si="0"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="K63" s="47">
         <f t="shared" si="8"/>
         <v>8.75</v>
       </c>
-      <c r="L63" s="26"/>
+      <c r="L63" s="49"/>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A64" s="2">
@@ -3376,21 +3396,21 @@
       <c r="G64" s="12">
         <v>10</v>
       </c>
-      <c r="H64" s="27">
-        <v>10</v>
-      </c>
-      <c r="I64" s="33" t="s">
-        <v>99</v>
-      </c>
-      <c r="J64" s="35">
-        <f t="shared" si="0"/>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="K64" s="35">
+      <c r="H64" s="26">
+        <v>10</v>
+      </c>
+      <c r="I64" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="J64" s="33">
+        <f t="shared" si="0"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="K64" s="47">
         <f t="shared" si="8"/>
         <v>8.75</v>
       </c>
-      <c r="L64" s="26"/>
+      <c r="L64" s="49"/>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A65" s="2">
@@ -3414,21 +3434,21 @@
       <c r="G65" s="12">
         <v>10</v>
       </c>
-      <c r="H65" s="27">
-        <v>10</v>
-      </c>
-      <c r="I65" s="33" t="s">
-        <v>99</v>
-      </c>
-      <c r="J65" s="35">
-        <f t="shared" si="0"/>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="K65" s="35">
+      <c r="H65" s="26">
+        <v>10</v>
+      </c>
+      <c r="I65" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="J65" s="33">
+        <f t="shared" si="0"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="K65" s="47">
         <f t="shared" si="8"/>
         <v>8.75</v>
       </c>
-      <c r="L65" s="26"/>
+      <c r="L65" s="49"/>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A66" s="2">
@@ -3452,21 +3472,21 @@
       <c r="G66" s="12">
         <v>10</v>
       </c>
-      <c r="H66" s="27">
-        <v>10</v>
-      </c>
-      <c r="I66" s="33" t="s">
-        <v>99</v>
-      </c>
-      <c r="J66" s="35">
-        <f t="shared" si="0"/>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="K66" s="35">
+      <c r="H66" s="26">
+        <v>10</v>
+      </c>
+      <c r="I66" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="J66" s="33">
+        <f t="shared" si="0"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="K66" s="47">
         <f t="shared" si="8"/>
         <v>8.75</v>
       </c>
-      <c r="L66" s="26"/>
+      <c r="L66" s="49"/>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A67" s="2">
@@ -3490,21 +3510,21 @@
       <c r="G67" s="12">
         <v>10</v>
       </c>
-      <c r="H67" s="27">
-        <v>10</v>
-      </c>
-      <c r="I67" s="33" t="s">
-        <v>99</v>
-      </c>
-      <c r="J67" s="35">
+      <c r="H67" s="26">
+        <v>10</v>
+      </c>
+      <c r="I67" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="J67" s="33">
         <f t="shared" ref="J67:J70" si="9">H67/60</f>
         <v>0.16666666666666666</v>
       </c>
-      <c r="K67" s="35">
+      <c r="K67" s="47">
         <f t="shared" si="8"/>
         <v>8.75</v>
       </c>
-      <c r="L67" s="26"/>
+      <c r="L67" s="49"/>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A68" s="2">
@@ -3528,21 +3548,21 @@
       <c r="G68" s="12">
         <v>20</v>
       </c>
-      <c r="H68" s="27">
+      <c r="H68" s="26">
         <v>30</v>
       </c>
-      <c r="I68" s="33" t="s">
+      <c r="I68" s="31" t="s">
         <v>98</v>
       </c>
-      <c r="J68" s="35">
+      <c r="J68" s="33">
         <f t="shared" si="9"/>
         <v>0.5</v>
       </c>
-      <c r="K68" s="35">
+      <c r="K68" s="47">
         <f>$O$2*J68</f>
         <v>37.5</v>
       </c>
-      <c r="L68" s="26"/>
+      <c r="L68" s="49"/>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A69" s="15">
@@ -3566,21 +3586,21 @@
       <c r="G69" s="18">
         <v>20</v>
       </c>
-      <c r="H69" s="29">
+      <c r="H69" s="28">
         <v>30</v>
       </c>
-      <c r="I69" s="33" t="s">
+      <c r="I69" s="31" t="s">
         <v>98</v>
       </c>
-      <c r="J69" s="35">
+      <c r="J69" s="33">
         <f t="shared" si="9"/>
         <v>0.5</v>
       </c>
-      <c r="K69" s="35">
+      <c r="K69" s="47">
         <f>$O$2*J69</f>
         <v>37.5</v>
       </c>
-      <c r="L69" s="26"/>
+      <c r="L69" s="49"/>
     </row>
     <row r="70" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A70" s="19">
@@ -3596,27 +3616,29 @@
       <c r="E70" s="22" t="s">
         <v>102</v>
       </c>
-      <c r="F70" s="47" t="s">
+      <c r="F70" s="45" t="s">
         <v>112</v>
       </c>
       <c r="G70" s="23">
         <v>30</v>
       </c>
-      <c r="H70" s="30">
+      <c r="H70" s="29">
         <v>480</v>
       </c>
-      <c r="I70" s="34" t="s">
+      <c r="I70" s="32" t="s">
         <v>106</v>
       </c>
-      <c r="J70" s="35">
+      <c r="J70" s="33">
         <f t="shared" si="9"/>
         <v>8</v>
       </c>
-      <c r="K70" s="35">
+      <c r="K70" s="47">
         <f>O3*J70</f>
         <v>420</v>
       </c>
-      <c r="L70" s="26"/>
+      <c r="L70" s="49">
+        <v>120</v>
+      </c>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.2">
       <c r="G71" s="14">
@@ -3625,7 +3647,7 @@
       </c>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="F72" s="37" t="s">
+      <c r="F72" s="35" t="s">
         <v>110</v>
       </c>
       <c r="G72" s="24">

</xml_diff>

<commit_message>
Acessibilidade: Ajuste nos icones de midia social
</commit_message>
<xml_diff>
--- a/documento_projeto/Pixels - Orçamento de correção.xlsx
+++ b/documento_projeto/Pixels - Orçamento de correção.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\pixels\documento_projeto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Fatec\pixels\documento_projeto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E63802C-DACC-47D2-8D95-2DE3CC99E47D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1190DB3D-8491-4D1D-BFB8-7697C06ABED2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2220" yWindow="2835" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="orçamento" sheetId="4" r:id="rId1"/>
@@ -399,21 +399,25 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Cambria"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Cambria"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Cambria"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -559,7 +563,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -696,6 +700,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -920,8 +930,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A045B8F-3550-4BE9-82FC-AF0F1FC4BEDF}">
   <dimension ref="A1:O72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F49" workbookViewId="0">
-      <selection activeCell="M70" sqref="M70"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1068,7 +1078,9 @@
         <f>O4*J3</f>
         <v>52.5</v>
       </c>
-      <c r="L3" s="49"/>
+      <c r="L3" s="49">
+        <v>50</v>
+      </c>
       <c r="N3" s="39" t="s">
         <v>106</v>
       </c>
@@ -1112,7 +1124,9 @@
         <f>O5*J4</f>
         <v>10</v>
       </c>
-      <c r="L4" s="49"/>
+      <c r="L4" s="49">
+        <v>10</v>
+      </c>
       <c r="N4" s="40" t="s">
         <v>99</v>
       </c>
@@ -1156,7 +1170,9 @@
         <f>O6*J5</f>
         <v>14.25</v>
       </c>
-      <c r="L5" s="49"/>
+      <c r="L5" s="49">
+        <v>18</v>
+      </c>
       <c r="N5" s="40" t="s">
         <v>104</v>
       </c>
@@ -1200,7 +1216,9 @@
         <f>O3*J6</f>
         <v>17.5</v>
       </c>
-      <c r="L6" s="49"/>
+      <c r="L6" s="49">
+        <v>2</v>
+      </c>
       <c r="N6" s="19" t="s">
         <v>105</v>
       </c>
@@ -1218,7 +1236,7 @@
       <c r="C7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="50" t="s">
         <v>24</v>
       </c>
       <c r="E7" s="5" t="s">
@@ -1244,7 +1262,9 @@
         <f>O2*J7</f>
         <v>12.5</v>
       </c>
-      <c r="L7" s="49"/>
+      <c r="L7" s="51">
+        <v>20</v>
+      </c>
     </row>
     <row r="8" spans="1:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2">

</xml_diff>

<commit_message>
Atualização das Planilhas de Execução
atualização das Planilhas de Execução
</commit_message>
<xml_diff>
--- a/documento_projeto/Pixels - Orçamento de correção.xlsx
+++ b/documento_projeto/Pixels - Orçamento de correção.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Fatec\pixels\documento_projeto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LUCASSILVESTREPAULA\Documents\GitHub\PIXELS\documento_projeto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1190DB3D-8491-4D1D-BFB8-7697C06ABED2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B46AD1AF-B1AA-486B-9A60-BC5A32EB34A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2220" yWindow="2835" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="orçamento" sheetId="4" r:id="rId1"/>
@@ -23,7 +23,6 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -930,8 +929,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A045B8F-3550-4BE9-82FC-AF0F1FC4BEDF}">
   <dimension ref="A1:O72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView tabSelected="1" topLeftCell="F31" workbookViewId="0">
+      <selection activeCell="L50" sqref="L50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1302,7 +1301,9 @@
         <f>$O$4*J8</f>
         <v>8.75</v>
       </c>
-      <c r="L8" s="49"/>
+      <c r="L8" s="49">
+        <v>10</v>
+      </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
@@ -1340,7 +1341,9 @@
         <f t="shared" ref="K9:K21" si="1">$O$4*J9</f>
         <v>8.75</v>
       </c>
-      <c r="L9" s="49"/>
+      <c r="L9" s="49">
+        <v>10</v>
+      </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
@@ -1378,7 +1381,9 @@
         <f t="shared" si="1"/>
         <v>8.75</v>
       </c>
-      <c r="L10" s="49"/>
+      <c r="L10" s="49">
+        <v>10</v>
+      </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
@@ -1416,7 +1421,9 @@
         <f t="shared" si="1"/>
         <v>8.75</v>
       </c>
-      <c r="L11" s="49"/>
+      <c r="L11" s="49">
+        <v>10</v>
+      </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
@@ -1454,7 +1461,9 @@
         <f t="shared" si="1"/>
         <v>8.75</v>
       </c>
-      <c r="L12" s="49"/>
+      <c r="L12" s="49">
+        <v>10</v>
+      </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
@@ -1492,7 +1501,9 @@
         <f t="shared" si="1"/>
         <v>8.75</v>
       </c>
-      <c r="L13" s="49"/>
+      <c r="L13" s="49">
+        <v>10</v>
+      </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
@@ -1530,7 +1541,9 @@
         <f t="shared" si="1"/>
         <v>8.75</v>
       </c>
-      <c r="L14" s="49"/>
+      <c r="L14" s="49">
+        <v>10</v>
+      </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
@@ -1568,7 +1581,9 @@
         <f t="shared" si="1"/>
         <v>8.75</v>
       </c>
-      <c r="L15" s="49"/>
+      <c r="L15" s="49">
+        <v>10</v>
+      </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
@@ -1606,7 +1621,9 @@
         <f t="shared" si="1"/>
         <v>8.75</v>
       </c>
-      <c r="L16" s="49"/>
+      <c r="L16" s="49">
+        <v>10</v>
+      </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
@@ -1644,7 +1661,9 @@
         <f t="shared" si="1"/>
         <v>8.75</v>
       </c>
-      <c r="L17" s="49"/>
+      <c r="L17" s="49">
+        <v>10</v>
+      </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
@@ -1682,7 +1701,9 @@
         <f t="shared" si="1"/>
         <v>8.75</v>
       </c>
-      <c r="L18" s="49"/>
+      <c r="L18" s="49">
+        <v>10</v>
+      </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
@@ -1720,7 +1741,9 @@
         <f t="shared" si="1"/>
         <v>8.75</v>
       </c>
-      <c r="L19" s="49"/>
+      <c r="L19" s="49">
+        <v>10</v>
+      </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
@@ -1758,7 +1781,9 @@
         <f t="shared" si="1"/>
         <v>8.75</v>
       </c>
-      <c r="L20" s="49"/>
+      <c r="L20" s="49">
+        <v>10</v>
+      </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
@@ -1796,7 +1821,9 @@
         <f t="shared" si="1"/>
         <v>8.75</v>
       </c>
-      <c r="L21" s="49"/>
+      <c r="L21" s="49">
+        <v>10</v>
+      </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
@@ -2024,7 +2051,9 @@
         <f>$O$4*J27</f>
         <v>8.75</v>
       </c>
-      <c r="L27" s="49"/>
+      <c r="L27" s="49">
+        <v>10</v>
+      </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
@@ -2062,7 +2091,9 @@
         <f t="shared" ref="K28:K30" si="3">$O$4*J28</f>
         <v>8.75</v>
       </c>
-      <c r="L28" s="49"/>
+      <c r="L28" s="49">
+        <v>10</v>
+      </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
@@ -2100,7 +2131,9 @@
         <f t="shared" si="3"/>
         <v>8.75</v>
       </c>
-      <c r="L29" s="49"/>
+      <c r="L29" s="49">
+        <v>10</v>
+      </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
@@ -2138,7 +2171,9 @@
         <f t="shared" si="3"/>
         <v>8.75</v>
       </c>
-      <c r="L30" s="49"/>
+      <c r="L30" s="49">
+        <v>10</v>
+      </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
@@ -3050,7 +3085,9 @@
         <f t="shared" si="8"/>
         <v>8.75</v>
       </c>
-      <c r="L54" s="49"/>
+      <c r="L54" s="49">
+        <v>10</v>
+      </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
@@ -3088,7 +3125,9 @@
         <f t="shared" si="8"/>
         <v>8.75</v>
       </c>
-      <c r="L55" s="49"/>
+      <c r="L55" s="49">
+        <v>10</v>
+      </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
@@ -3126,7 +3165,9 @@
         <f t="shared" si="8"/>
         <v>8.75</v>
       </c>
-      <c r="L56" s="49"/>
+      <c r="L56" s="49">
+        <v>10</v>
+      </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
@@ -3164,7 +3205,9 @@
         <f t="shared" si="8"/>
         <v>8.75</v>
       </c>
-      <c r="L57" s="49"/>
+      <c r="L57" s="49">
+        <v>10</v>
+      </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
@@ -3202,7 +3245,9 @@
         <f t="shared" si="8"/>
         <v>8.75</v>
       </c>
-      <c r="L58" s="49"/>
+      <c r="L58" s="49">
+        <v>10</v>
+      </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
@@ -3240,7 +3285,9 @@
         <f t="shared" si="8"/>
         <v>8.75</v>
       </c>
-      <c r="L59" s="49"/>
+      <c r="L59" s="49">
+        <v>10</v>
+      </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A60" s="2">
@@ -3278,7 +3325,9 @@
         <f t="shared" si="8"/>
         <v>8.75</v>
       </c>
-      <c r="L60" s="49"/>
+      <c r="L60" s="49">
+        <v>10</v>
+      </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A61" s="2">
@@ -3316,7 +3365,9 @@
         <f t="shared" si="8"/>
         <v>8.75</v>
       </c>
-      <c r="L61" s="49"/>
+      <c r="L61" s="49">
+        <v>10</v>
+      </c>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A62" s="2">
@@ -3354,7 +3405,9 @@
         <f t="shared" si="8"/>
         <v>8.75</v>
       </c>
-      <c r="L62" s="49"/>
+      <c r="L62" s="49">
+        <v>10</v>
+      </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A63" s="2">
@@ -3392,7 +3445,9 @@
         <f t="shared" si="8"/>
         <v>8.75</v>
       </c>
-      <c r="L63" s="49"/>
+      <c r="L63" s="49">
+        <v>10</v>
+      </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A64" s="2">
@@ -3430,7 +3485,9 @@
         <f t="shared" si="8"/>
         <v>8.75</v>
       </c>
-      <c r="L64" s="49"/>
+      <c r="L64" s="49">
+        <v>10</v>
+      </c>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A65" s="2">
@@ -3468,7 +3525,9 @@
         <f t="shared" si="8"/>
         <v>8.75</v>
       </c>
-      <c r="L65" s="49"/>
+      <c r="L65" s="49">
+        <v>10</v>
+      </c>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A66" s="2">
@@ -3506,7 +3565,9 @@
         <f t="shared" si="8"/>
         <v>8.75</v>
       </c>
-      <c r="L66" s="49"/>
+      <c r="L66" s="49">
+        <v>10</v>
+      </c>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A67" s="2">
@@ -3544,7 +3605,9 @@
         <f t="shared" si="8"/>
         <v>8.75</v>
       </c>
-      <c r="L67" s="49"/>
+      <c r="L67" s="49">
+        <v>10</v>
+      </c>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A68" s="2">

</xml_diff>